<commit_message>
integarate MR profile for anonymization
</commit_message>
<xml_diff>
--- a/shanoir-ng-import/src/main/resources/anonymization.xlsx
+++ b/shanoir-ng-import/src/main/resources/anonymization.xlsx
@@ -3,16 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ifakhfak\Documents\Shanoir NG\Import MS\Anomymization Spec\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17325" windowHeight="7575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A261:G283"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="821">
   <si>
     <t>Attribute Name</t>
   </si>
@@ -2372,12 +2376,6 @@
   </si>
   <si>
     <t>C.7.5.1</t>
-  </si>
-  <si>
-    <t>Device</t>
-  </si>
-  <si>
-    <t>C.7.6.12</t>
   </si>
   <si>
     <t>SOP Common</t>
@@ -2626,6 +2624,9 @@
   </si>
   <si>
     <t>Z ?</t>
+  </si>
+  <si>
+    <t>MR Profile</t>
   </si>
 </sst>
 </file>
@@ -2767,7 +2768,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2847,6 +2848,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent2" xfId="3" builtinId="33"/>
@@ -3138,10 +3142,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D305"/>
+  <dimension ref="A1:E305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A261" workbookViewId="0">
-      <selection activeCell="A316" sqref="A316"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3150,9 +3154,10 @@
     <col min="2" max="2" width="18.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3165,8 +3170,11 @@
       <c r="D1" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="33" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -3179,8 +3187,11 @@
       <c r="D4" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>410</v>
       </c>
@@ -3193,8 +3204,11 @@
       <c r="D5" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>411</v>
       </c>
@@ -3207,8 +3221,11 @@
       <c r="D6" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>13</v>
       </c>
@@ -3221,8 +3238,11 @@
       <c r="D7" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>412</v>
       </c>
@@ -3235,8 +3255,11 @@
       <c r="D8" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>413</v>
       </c>
@@ -3249,8 +3272,11 @@
       <c r="D9" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>414</v>
       </c>
@@ -3263,8 +3289,11 @@
       <c r="D10" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -3277,8 +3306,11 @@
       <c r="D11" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>415</v>
       </c>
@@ -3291,8 +3323,11 @@
       <c r="D12" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>416</v>
       </c>
@@ -3305,8 +3340,11 @@
       <c r="D13" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -3319,8 +3357,11 @@
       <c r="D14" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>23</v>
       </c>
@@ -3333,18 +3374,23 @@
       <c r="D15" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>417</v>
       </c>
@@ -3357,8 +3403,11 @@
       <c r="D18" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>418</v>
       </c>
@@ -3371,8 +3420,11 @@
       <c r="D19" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -3385,8 +3437,11 @@
       <c r="D20" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>419</v>
       </c>
@@ -3399,8 +3454,11 @@
       <c r="D21" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -3413,8 +3471,11 @@
       <c r="D22" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -3427,8 +3488,11 @@
       <c r="D23" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>420</v>
       </c>
@@ -3441,8 +3505,11 @@
       <c r="D24" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -3455,8 +3522,11 @@
       <c r="D25" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -3469,8 +3539,11 @@
       <c r="D26" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>421</v>
       </c>
@@ -3483,8 +3556,11 @@
       <c r="D27" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -3497,8 +3573,11 @@
       <c r="D28" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>422</v>
       </c>
@@ -3511,23 +3590,29 @@
       <c r="D29" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="9"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="9"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>423</v>
       </c>
@@ -3540,8 +3625,11 @@
       <c r="D33" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>424</v>
       </c>
@@ -3554,8 +3642,11 @@
       <c r="D34" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -3568,8 +3659,11 @@
       <c r="D35" s="9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -3582,8 +3676,11 @@
       <c r="D36" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -3596,8 +3693,11 @@
       <c r="D37" s="9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>425</v>
       </c>
@@ -3610,8 +3710,11 @@
       <c r="D38" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>426</v>
       </c>
@@ -3624,8 +3727,11 @@
       <c r="D39" s="9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -3638,8 +3744,11 @@
       <c r="D40" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>427</v>
       </c>
@@ -3652,8 +3761,11 @@
       <c r="D41" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>428</v>
       </c>
@@ -3666,8 +3778,11 @@
       <c r="D42" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>59</v>
       </c>
@@ -3680,8 +3795,11 @@
       <c r="D43" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>61</v>
       </c>
@@ -3694,8 +3812,11 @@
       <c r="D44" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>63</v>
       </c>
@@ -3708,8 +3829,11 @@
       <c r="D45" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>65</v>
       </c>
@@ -3722,23 +3846,29 @@
       <c r="D46" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="9"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B48" s="4"/>
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="9"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B49" s="4"/>
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="9"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>429</v>
       </c>
@@ -3751,8 +3881,11 @@
       <c r="D50" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>68</v>
       </c>
@@ -3765,8 +3898,11 @@
       <c r="D51" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>70</v>
       </c>
@@ -3779,8 +3915,11 @@
       <c r="D52" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>72</v>
       </c>
@@ -3793,8 +3932,11 @@
       <c r="D53" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>74</v>
       </c>
@@ -3807,8 +3949,11 @@
       <c r="D54" s="9" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>77</v>
       </c>
@@ -3821,8 +3966,11 @@
       <c r="D55" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>430</v>
       </c>
@@ -3835,8 +3983,11 @@
       <c r="D56" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>431</v>
       </c>
@@ -3849,8 +4000,11 @@
       <c r="D57" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>432</v>
       </c>
@@ -3863,8 +4017,11 @@
       <c r="D58" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>82</v>
       </c>
@@ -3877,8 +4034,11 @@
       <c r="D59" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>84</v>
       </c>
@@ -3891,8 +4051,11 @@
       <c r="D60" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>86</v>
       </c>
@@ -3905,18 +4068,23 @@
       <c r="D61" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B62" s="4"/>
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" s="9"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B63" s="4"/>
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" s="9"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>433</v>
       </c>
@@ -3929,8 +4097,11 @@
       <c r="D64" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>89</v>
       </c>
@@ -3943,8 +4114,11 @@
       <c r="D65" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>434</v>
       </c>
@@ -3957,8 +4131,11 @@
       <c r="D66" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>92</v>
       </c>
@@ -3971,8 +4148,11 @@
       <c r="D67" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>94</v>
       </c>
@@ -3985,8 +4165,11 @@
       <c r="D68" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>96</v>
       </c>
@@ -3999,8 +4182,11 @@
       <c r="D69" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>435</v>
       </c>
@@ -4013,8 +4199,11 @@
       <c r="D70" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>99</v>
       </c>
@@ -4027,8 +4216,11 @@
       <c r="D71" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>101</v>
       </c>
@@ -4041,8 +4233,11 @@
       <c r="D72" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>103</v>
       </c>
@@ -4055,8 +4250,11 @@
       <c r="D73" s="9" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>106</v>
       </c>
@@ -4069,8 +4267,11 @@
       <c r="D74" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>108</v>
       </c>
@@ -4083,23 +4284,29 @@
       <c r="D75" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B76" s="4"/>
       <c r="C76" s="9"/>
       <c r="D76" s="9"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" s="9"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B77" s="4"/>
       <c r="C77" s="9"/>
       <c r="D77" s="9"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" s="9"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B78" s="4"/>
       <c r="C78" s="9"/>
       <c r="D78" s="9"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" s="9"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>110</v>
       </c>
@@ -4112,8 +4319,11 @@
       <c r="D79" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>112</v>
       </c>
@@ -4126,8 +4336,11 @@
       <c r="D80" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>114</v>
       </c>
@@ -4140,8 +4353,11 @@
       <c r="D81" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>116</v>
       </c>
@@ -4154,8 +4370,11 @@
       <c r="D82" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>436</v>
       </c>
@@ -4168,8 +4387,11 @@
       <c r="D83" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>119</v>
       </c>
@@ -4182,8 +4404,11 @@
       <c r="D84" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>122</v>
       </c>
@@ -4196,8 +4421,11 @@
       <c r="D85" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>124</v>
       </c>
@@ -4210,8 +4438,11 @@
       <c r="D86" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E86" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>126</v>
       </c>
@@ -4224,8 +4455,11 @@
       <c r="D87" s="9" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>128</v>
       </c>
@@ -4238,8 +4472,11 @@
       <c r="D88" s="9" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E88" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>130</v>
       </c>
@@ -4252,8 +4489,11 @@
       <c r="D89" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>132</v>
       </c>
@@ -4266,23 +4506,29 @@
       <c r="D90" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B91" s="4"/>
       <c r="C91" s="9"/>
       <c r="D91" s="9"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91" s="9"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B92" s="4"/>
       <c r="C92" s="9"/>
       <c r="D92" s="9"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92" s="9"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B93" s="4"/>
       <c r="C93" s="9"/>
       <c r="D93" s="9"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93" s="9"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>437</v>
       </c>
@@ -4295,8 +4541,11 @@
       <c r="D94" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>135</v>
       </c>
@@ -4309,8 +4558,11 @@
       <c r="D95" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>137</v>
       </c>
@@ -4323,8 +4575,11 @@
       <c r="D96" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>139</v>
       </c>
@@ -4337,8 +4592,11 @@
       <c r="D97" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="17" t="s">
         <v>141</v>
       </c>
@@ -4351,8 +4609,11 @@
       <c r="D98" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>438</v>
       </c>
@@ -4365,8 +4626,11 @@
       <c r="D99" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>144</v>
       </c>
@@ -4379,8 +4643,11 @@
       <c r="D100" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>146</v>
       </c>
@@ -4393,8 +4660,11 @@
       <c r="D101" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>439</v>
       </c>
@@ -4407,8 +4677,11 @@
       <c r="D102" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>440</v>
       </c>
@@ -4421,8 +4694,11 @@
       <c r="D103" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>150</v>
       </c>
@@ -4435,23 +4711,29 @@
       <c r="D104" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B105" s="4"/>
       <c r="C105" s="9"/>
       <c r="D105" s="9"/>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105" s="9"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B106" s="4"/>
       <c r="C106" s="9"/>
       <c r="D106" s="9"/>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106" s="9"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B107" s="4"/>
       <c r="C107" s="9"/>
       <c r="D107" s="9"/>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107" s="9"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>441</v>
       </c>
@@ -4464,8 +4746,11 @@
       <c r="D108" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>153</v>
       </c>
@@ -4478,8 +4763,11 @@
       <c r="D109" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>155</v>
       </c>
@@ -4492,8 +4780,11 @@
       <c r="D110" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>157</v>
       </c>
@@ -4506,8 +4797,11 @@
       <c r="D111" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>160</v>
       </c>
@@ -4520,8 +4814,11 @@
       <c r="D112" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E112" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>162</v>
       </c>
@@ -4534,8 +4831,11 @@
       <c r="D113" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E113" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>442</v>
       </c>
@@ -4548,8 +4848,11 @@
       <c r="D114" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E114" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>165</v>
       </c>
@@ -4562,8 +4865,11 @@
       <c r="D115" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E115" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>443</v>
       </c>
@@ -4576,8 +4882,11 @@
       <c r="D116" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E116" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>168</v>
       </c>
@@ -4590,8 +4899,11 @@
       <c r="D117" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E117" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>170</v>
       </c>
@@ -4604,8 +4916,11 @@
       <c r="D118" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E118" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>444</v>
       </c>
@@ -4618,23 +4933,29 @@
       <c r="D119" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E119" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B120" s="4"/>
       <c r="C120" s="9"/>
       <c r="D120" s="9"/>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E120" s="9"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B121" s="4"/>
       <c r="C121" s="9"/>
       <c r="D121" s="9"/>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E121" s="9"/>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B122" s="4"/>
       <c r="C122" s="9"/>
       <c r="D122" s="9"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E122" s="9"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>445</v>
       </c>
@@ -4647,8 +4968,11 @@
       <c r="D123" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E123" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>174</v>
       </c>
@@ -4661,8 +4985,11 @@
       <c r="D124" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E124" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>176</v>
       </c>
@@ -4675,8 +5002,11 @@
       <c r="D125" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E125" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>178</v>
       </c>
@@ -4689,8 +5019,11 @@
       <c r="D126" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E126" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>180</v>
       </c>
@@ -4703,8 +5036,11 @@
       <c r="D127" s="9" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E127" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>446</v>
       </c>
@@ -4717,8 +5053,11 @@
       <c r="D128" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E128" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>183</v>
       </c>
@@ -4731,8 +5070,11 @@
       <c r="D129" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E129" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>185</v>
       </c>
@@ -4745,8 +5087,11 @@
       <c r="D130" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E130" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>187</v>
       </c>
@@ -4759,8 +5104,11 @@
       <c r="D131" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E131" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>189</v>
       </c>
@@ -4773,8 +5121,11 @@
       <c r="D132" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E132" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>191</v>
       </c>
@@ -4787,8 +5138,11 @@
       <c r="D133" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E133" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>193</v>
       </c>
@@ -4801,23 +5155,29 @@
       <c r="D134" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E134" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B135" s="4"/>
       <c r="C135" s="9"/>
       <c r="D135" s="9"/>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E135" s="9"/>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B136" s="4"/>
       <c r="C136" s="9"/>
       <c r="D136" s="9"/>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E136" s="9"/>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B137" s="4"/>
       <c r="C137" s="9"/>
       <c r="D137" s="9"/>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E137" s="9"/>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>644</v>
       </c>
@@ -4830,8 +5190,11 @@
       <c r="D138" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E138" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>196</v>
       </c>
@@ -4844,8 +5207,11 @@
       <c r="D139" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E139" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>198</v>
       </c>
@@ -4858,8 +5224,11 @@
       <c r="D140" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E140" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>200</v>
       </c>
@@ -4872,8 +5241,11 @@
       <c r="D141" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E141" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>202</v>
       </c>
@@ -4886,8 +5258,11 @@
       <c r="D142" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E142" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>204</v>
       </c>
@@ -4900,8 +5275,11 @@
       <c r="D143" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E143" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>206</v>
       </c>
@@ -4914,8 +5292,11 @@
       <c r="D144" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E144" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>208</v>
       </c>
@@ -4928,8 +5309,11 @@
       <c r="D145" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E145" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>210</v>
       </c>
@@ -4942,8 +5326,11 @@
       <c r="D146" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E146" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="17" t="s">
         <v>212</v>
       </c>
@@ -4956,8 +5343,11 @@
       <c r="D147" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E147" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>214</v>
       </c>
@@ -4970,8 +5360,11 @@
       <c r="D148" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E148" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>447</v>
       </c>
@@ -4984,8 +5377,11 @@
       <c r="D149" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E149" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="14" t="s">
         <v>217</v>
       </c>
@@ -4998,8 +5394,11 @@
       <c r="D150" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E150" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>219</v>
       </c>
@@ -5012,8 +5411,11 @@
       <c r="D151" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E151" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>448</v>
       </c>
@@ -5026,8 +5428,11 @@
       <c r="D152" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E152" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>222</v>
       </c>
@@ -5040,23 +5445,29 @@
       <c r="D153" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E153" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B154" s="4"/>
       <c r="C154" s="9"/>
       <c r="D154" s="9"/>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E154" s="9"/>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B155" s="4"/>
       <c r="C155" s="9"/>
       <c r="D155" s="9"/>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E155" s="9"/>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B156" s="4"/>
       <c r="C156" s="9"/>
       <c r="D156" s="9"/>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E156" s="9"/>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>449</v>
       </c>
@@ -5069,8 +5480,11 @@
       <c r="D157" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E157" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>450</v>
       </c>
@@ -5083,8 +5497,11 @@
       <c r="D158" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E158" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>451</v>
       </c>
@@ -5097,8 +5514,11 @@
       <c r="D159" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E159" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>227</v>
       </c>
@@ -5111,8 +5531,11 @@
       <c r="D160" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E160" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>452</v>
       </c>
@@ -5125,8 +5548,11 @@
       <c r="D161" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E161" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>453</v>
       </c>
@@ -5139,8 +5565,11 @@
       <c r="D162" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E162" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>454</v>
       </c>
@@ -5153,8 +5582,11 @@
       <c r="D163" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E163" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="14" t="s">
         <v>232</v>
       </c>
@@ -5167,8 +5599,11 @@
       <c r="D164" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E164" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="14" t="s">
         <v>234</v>
       </c>
@@ -5181,8 +5616,11 @@
       <c r="D165" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E165" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>455</v>
       </c>
@@ -5195,8 +5633,11 @@
       <c r="D166" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E166" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="14" t="s">
         <v>237</v>
       </c>
@@ -5209,8 +5650,11 @@
       <c r="D167" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E167" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>456</v>
       </c>
@@ -5223,18 +5667,23 @@
       <c r="D168" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E168" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B169" s="4"/>
       <c r="C169" s="9"/>
       <c r="D169" s="9"/>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E169" s="9"/>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B170" s="4"/>
       <c r="C170" s="9"/>
       <c r="D170" s="9"/>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E170" s="9"/>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>457</v>
       </c>
@@ -5247,8 +5696,11 @@
       <c r="D171" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E171" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>241</v>
       </c>
@@ -5261,8 +5713,11 @@
       <c r="D172" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E172" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>458</v>
       </c>
@@ -5275,8 +5730,11 @@
       <c r="D173" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E173" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>459</v>
       </c>
@@ -5289,8 +5747,11 @@
       <c r="D174" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E174" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>460</v>
       </c>
@@ -5303,8 +5764,11 @@
       <c r="D175" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E175" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>461</v>
       </c>
@@ -5317,8 +5781,11 @@
       <c r="D176" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E176" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>462</v>
       </c>
@@ -5331,8 +5798,11 @@
       <c r="D177" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E177" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>463</v>
       </c>
@@ -5345,8 +5815,11 @@
       <c r="D178" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E178" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>464</v>
       </c>
@@ -5359,23 +5832,29 @@
       <c r="D179" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E179" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B180" s="4"/>
       <c r="C180" s="9"/>
       <c r="D180" s="9"/>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E180" s="9"/>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B181" s="4"/>
       <c r="C181" s="9"/>
       <c r="D181" s="9"/>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E181" s="9"/>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B182" s="4"/>
       <c r="C182" s="9"/>
       <c r="D182" s="9"/>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E182" s="9"/>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>465</v>
       </c>
@@ -5388,8 +5867,11 @@
       <c r="D183" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E183" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>251</v>
       </c>
@@ -5402,8 +5884,11 @@
       <c r="D184" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E184" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>253</v>
       </c>
@@ -5416,8 +5901,11 @@
       <c r="D185" s="9" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E185" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>255</v>
       </c>
@@ -5430,8 +5918,11 @@
       <c r="D186" s="9" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E186" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>466</v>
       </c>
@@ -5444,8 +5935,11 @@
       <c r="D187" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E187" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>467</v>
       </c>
@@ -5458,8 +5952,11 @@
       <c r="D188" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E188" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>468</v>
       </c>
@@ -5472,8 +5969,11 @@
       <c r="D189" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E189" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>260</v>
       </c>
@@ -5486,8 +5986,11 @@
       <c r="D190" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E190" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>262</v>
       </c>
@@ -5500,8 +6003,11 @@
       <c r="D191" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E191" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>469</v>
       </c>
@@ -5514,23 +6020,29 @@
       <c r="D192" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E192" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B193" s="4"/>
       <c r="C193" s="9"/>
       <c r="D193" s="9"/>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E193" s="9"/>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B194" s="4"/>
       <c r="C194" s="9"/>
       <c r="D194" s="9"/>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E194" s="9"/>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B195" s="4"/>
       <c r="C195" s="9"/>
       <c r="D195" s="9"/>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E195" s="9"/>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>265</v>
       </c>
@@ -5543,8 +6055,11 @@
       <c r="D196" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E196" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>267</v>
       </c>
@@ -5557,8 +6072,11 @@
       <c r="D197" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E197" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>269</v>
       </c>
@@ -5571,8 +6089,11 @@
       <c r="D198" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="199" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E198" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>271</v>
       </c>
@@ -5585,8 +6106,11 @@
       <c r="D199" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E199" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>273</v>
       </c>
@@ -5599,8 +6123,11 @@
       <c r="D200" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E200" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>275</v>
       </c>
@@ -5613,8 +6140,11 @@
       <c r="D201" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E201" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>277</v>
       </c>
@@ -5627,8 +6157,11 @@
       <c r="D202" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E202" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>470</v>
       </c>
@@ -5641,8 +6174,11 @@
       <c r="D203" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E203" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>471</v>
       </c>
@@ -5655,8 +6191,11 @@
       <c r="D204" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="205" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E204" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>472</v>
       </c>
@@ -5669,8 +6208,11 @@
       <c r="D205" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E205" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>473</v>
       </c>
@@ -5683,23 +6225,29 @@
       <c r="D206" s="9" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E206" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B207" s="4"/>
       <c r="C207" s="9"/>
       <c r="D207" s="9"/>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E207" s="9"/>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B208" s="4"/>
       <c r="C208" s="9"/>
       <c r="D208" s="9"/>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E208" s="9"/>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B209" s="4"/>
       <c r="C209" s="9"/>
       <c r="D209" s="9"/>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E209" s="9"/>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>474</v>
       </c>
@@ -5712,8 +6260,11 @@
       <c r="D210" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E210" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>475</v>
       </c>
@@ -5726,8 +6277,11 @@
       <c r="D211" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E211" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>476</v>
       </c>
@@ -5740,8 +6294,11 @@
       <c r="D212" s="9" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E212" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>287</v>
       </c>
@@ -5754,8 +6311,11 @@
       <c r="D213" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E213" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>477</v>
       </c>
@@ -5768,8 +6328,11 @@
       <c r="D214" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E214" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>478</v>
       </c>
@@ -5782,8 +6345,11 @@
       <c r="D215" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E215" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>479</v>
       </c>
@@ -5796,8 +6362,11 @@
       <c r="D216" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E216" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>480</v>
       </c>
@@ -5810,8 +6379,11 @@
       <c r="D217" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E217" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>481</v>
       </c>
@@ -5824,18 +6396,23 @@
       <c r="D218" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E218" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B219" s="4"/>
       <c r="C219" s="9"/>
       <c r="D219" s="9"/>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E219" s="9"/>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B220" s="4"/>
       <c r="C220" s="9"/>
       <c r="D220" s="9"/>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E220" s="9"/>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>482</v>
       </c>
@@ -5848,8 +6425,11 @@
       <c r="D221" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E221" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>483</v>
       </c>
@@ -5862,8 +6442,11 @@
       <c r="D222" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E222" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>296</v>
       </c>
@@ -5876,8 +6459,11 @@
       <c r="D223" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E223" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>298</v>
       </c>
@@ -5890,8 +6476,11 @@
       <c r="D224" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E224" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>484</v>
       </c>
@@ -5904,8 +6493,11 @@
       <c r="D225" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E225" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>485</v>
       </c>
@@ -5918,8 +6510,11 @@
       <c r="D226" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E226" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>486</v>
       </c>
@@ -5932,8 +6527,11 @@
       <c r="D227" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E227" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>303</v>
       </c>
@@ -5946,8 +6544,11 @@
       <c r="D228" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E228" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>487</v>
       </c>
@@ -5960,8 +6561,11 @@
       <c r="D229" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E229" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>488</v>
       </c>
@@ -5974,23 +6578,29 @@
       <c r="D230" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E230" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B231" s="4"/>
       <c r="C231" s="9"/>
       <c r="D231" s="9"/>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E231" s="9"/>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B232" s="4"/>
       <c r="C232" s="9"/>
       <c r="D232" s="9"/>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E232" s="9"/>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B233" s="4"/>
       <c r="C233" s="9"/>
       <c r="D233" s="9"/>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E233" s="9"/>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>489</v>
       </c>
@@ -6003,8 +6613,11 @@
       <c r="D234" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E234" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>490</v>
       </c>
@@ -6017,8 +6630,11 @@
       <c r="D235" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E235" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>491</v>
       </c>
@@ -6031,8 +6647,11 @@
       <c r="D236" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E236" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>492</v>
       </c>
@@ -6045,8 +6664,11 @@
       <c r="D237" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E237" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>493</v>
       </c>
@@ -6059,8 +6681,11 @@
       <c r="D238" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E238" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>312</v>
       </c>
@@ -6073,8 +6698,11 @@
       <c r="D239" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E239" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>314</v>
       </c>
@@ -6087,8 +6715,11 @@
       <c r="D240" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E240" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>316</v>
       </c>
@@ -6101,8 +6732,11 @@
       <c r="D241" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E241" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>318</v>
       </c>
@@ -6115,8 +6749,11 @@
       <c r="D242" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E242" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>494</v>
       </c>
@@ -6129,8 +6766,11 @@
       <c r="D243" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E243" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>495</v>
       </c>
@@ -6143,18 +6783,23 @@
       <c r="D244" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E244" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B245" s="4"/>
       <c r="C245" s="9"/>
       <c r="D245" s="9"/>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E245" s="9"/>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B246" s="4"/>
       <c r="C246" s="9"/>
       <c r="D246" s="9"/>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E246" s="9"/>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>496</v>
       </c>
@@ -6167,8 +6812,11 @@
       <c r="D247" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E247" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>497</v>
       </c>
@@ -6181,8 +6829,11 @@
       <c r="D248" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E248" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>498</v>
       </c>
@@ -6195,8 +6846,11 @@
       <c r="D249" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E249" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>325</v>
       </c>
@@ -6209,8 +6863,11 @@
       <c r="D250" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E250" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>499</v>
       </c>
@@ -6223,8 +6880,11 @@
       <c r="D251" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E251" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>500</v>
       </c>
@@ -6237,8 +6897,11 @@
       <c r="D252" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E252" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>501</v>
       </c>
@@ -6251,8 +6914,11 @@
       <c r="D253" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E253" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>330</v>
       </c>
@@ -6265,23 +6931,29 @@
       <c r="D254" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E254" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B255" s="4"/>
       <c r="C255" s="9"/>
       <c r="D255" s="9"/>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E255" s="9"/>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B256" s="4"/>
       <c r="C256" s="9"/>
       <c r="D256" s="9"/>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E256" s="9"/>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B257" s="4"/>
       <c r="C257" s="9"/>
       <c r="D257" s="9"/>
-    </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E257" s="9"/>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>502</v>
       </c>
@@ -6294,8 +6966,11 @@
       <c r="D258" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E258" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>503</v>
       </c>
@@ -6308,8 +6983,11 @@
       <c r="D259" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E259" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>334</v>
       </c>
@@ -6322,8 +7000,11 @@
       <c r="D260" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E260" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>336</v>
       </c>
@@ -6336,8 +7017,11 @@
       <c r="D261" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E261" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>338</v>
       </c>
@@ -6350,8 +7034,11 @@
       <c r="D262" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E262" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>340</v>
       </c>
@@ -6364,8 +7051,11 @@
       <c r="D263" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E263" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>342</v>
       </c>
@@ -6378,8 +7068,11 @@
       <c r="D264" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E264" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="14" t="s">
         <v>344</v>
       </c>
@@ -6392,8 +7085,11 @@
       <c r="D265" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E265" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>346</v>
       </c>
@@ -6406,8 +7102,11 @@
       <c r="D266" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E266" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="18" t="s">
         <v>348</v>
       </c>
@@ -6420,8 +7119,11 @@
       <c r="D267" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E267" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>504</v>
       </c>
@@ -6434,8 +7136,11 @@
       <c r="D268" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E268" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>351</v>
       </c>
@@ -6448,8 +7153,11 @@
       <c r="D269" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E269" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>353</v>
       </c>
@@ -6462,8 +7170,11 @@
       <c r="D270" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E270" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>159</v>
       </c>
@@ -6476,28 +7187,35 @@
       <c r="D271" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E271" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B272" s="4"/>
       <c r="C272" s="9"/>
       <c r="D272" s="9"/>
-    </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E272" s="9"/>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B273" s="4"/>
       <c r="C273" s="9"/>
       <c r="D273" s="9"/>
-    </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E273" s="9"/>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B274" s="4"/>
       <c r="C274" s="9"/>
       <c r="D274" s="9"/>
-    </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E274" s="9"/>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B275" s="4"/>
       <c r="C275" s="9"/>
       <c r="D275" s="9"/>
-    </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E275" s="9"/>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>356</v>
       </c>
@@ -6510,8 +7228,11 @@
       <c r="D276" s="9" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E276" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>358</v>
       </c>
@@ -6524,8 +7245,11 @@
       <c r="D277" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E277" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>360</v>
       </c>
@@ -6538,8 +7262,11 @@
       <c r="D278" s="9" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E278" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>505</v>
       </c>
@@ -6552,8 +7279,11 @@
       <c r="D279" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E279" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>363</v>
       </c>
@@ -6566,8 +7296,11 @@
       <c r="D280" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E280" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="14" t="s">
         <v>365</v>
       </c>
@@ -6580,8 +7313,11 @@
       <c r="D281" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E281" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="14" t="s">
         <v>367</v>
       </c>
@@ -6594,8 +7330,11 @@
       <c r="D282" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E282" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>369</v>
       </c>
@@ -6608,8 +7347,11 @@
       <c r="D283" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E283" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>371</v>
       </c>
@@ -6622,8 +7364,11 @@
       <c r="D284" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E284" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>373</v>
       </c>
@@ -6636,8 +7381,11 @@
       <c r="D285" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E285" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="18" t="s">
         <v>375</v>
       </c>
@@ -6650,8 +7398,11 @@
       <c r="D286" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E286" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>506</v>
       </c>
@@ -6664,8 +7415,11 @@
       <c r="D287" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E287" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>378</v>
       </c>
@@ -6678,8 +7432,11 @@
       <c r="D288" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E288" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>380</v>
       </c>
@@ -6692,8 +7449,11 @@
       <c r="D289" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E289" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>382</v>
       </c>
@@ -6706,18 +7466,23 @@
       <c r="D290" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E290" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B291" s="4"/>
       <c r="C291" s="9"/>
       <c r="D291" s="9"/>
-    </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E291" s="9"/>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B292" s="4"/>
       <c r="C292" s="9"/>
       <c r="D292" s="9"/>
-    </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E292" s="9"/>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>384</v>
       </c>
@@ -6730,8 +7495,11 @@
       <c r="D293" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E293" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>386</v>
       </c>
@@ -6744,8 +7512,11 @@
       <c r="D294" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E294" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>388</v>
       </c>
@@ -6758,8 +7529,11 @@
       <c r="D295" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E295" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>390</v>
       </c>
@@ -6772,8 +7546,11 @@
       <c r="D296" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E296" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>392</v>
       </c>
@@ -6786,8 +7563,11 @@
       <c r="D297" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E297" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>394</v>
       </c>
@@ -6800,8 +7580,11 @@
       <c r="D298" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E298" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>396</v>
       </c>
@@ -6814,8 +7597,11 @@
       <c r="D299" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E299" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>121</v>
       </c>
@@ -6828,8 +7614,11 @@
       <c r="D300" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E300" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>399</v>
       </c>
@@ -6842,8 +7631,11 @@
       <c r="D301" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E301" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>401</v>
       </c>
@@ -6856,8 +7648,11 @@
       <c r="D302" s="9" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E302" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>403</v>
       </c>
@@ -6870,8 +7665,11 @@
       <c r="D303" s="9" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E303" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>405</v>
       </c>
@@ -6884,8 +7682,11 @@
       <c r="D304" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E304" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>407</v>
       </c>
@@ -6896,6 +7697,9 @@
         <v>765</v>
       </c>
       <c r="D305" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E305" s="9" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7020,8 +7824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7065,10 +7869,10 @@
         <v>770</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -7100,7 +7904,7 @@
         <v>6</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -7132,7 +7936,7 @@
         <v>9</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -7158,7 +7962,7 @@
         <v>9</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -7190,7 +7994,7 @@
         <v>6</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -7219,13 +8023,13 @@
         <v>779</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>48</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -7254,13 +8058,13 @@
         <v>779</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>48</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -7292,7 +8096,7 @@
         <v>48</v>
       </c>
       <c r="K11" s="31" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -7324,46 +8128,30 @@
         <v>76</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="10"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
-      <c r="E13" s="28" t="s">
-        <v>782</v>
-      </c>
-      <c r="F13" s="28" t="s">
-        <v>783</v>
-      </c>
-      <c r="G13" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" s="4">
-        <v>3</v>
-      </c>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="4"/>
       <c r="J13" s="9"/>
       <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E14" s="28" t="s">
-        <v>784</v>
-      </c>
-      <c r="F14" s="28" t="s">
-        <v>785</v>
-      </c>
-      <c r="G14" s="28" t="s">
-        <v>774</v>
-      </c>
-      <c r="H14" s="4">
-        <v>3</v>
-      </c>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="4"/>
       <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>127</v>
@@ -7384,7 +8172,7 @@
         <v>76</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -7416,7 +8204,7 @@
         <v>76</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -7424,10 +8212,10 @@
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="28" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="G17" s="28" t="s">
         <v>774</v>
@@ -7452,10 +8240,10 @@
         <v>9</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="F18" s="28" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="G18" s="28" t="s">
         <v>774</v>
@@ -7467,7 +8255,7 @@
         <v>9</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -7475,10 +8263,10 @@
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="28" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>774</v>
@@ -7503,10 +8291,10 @@
         <v>76</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="G20" s="28" t="s">
         <v>774</v>
@@ -7518,7 +8306,7 @@
         <v>76</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -7526,10 +8314,10 @@
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="28" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="G21" s="28" t="s">
         <v>774</v>
@@ -7554,10 +8342,10 @@
         <v>6</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="G22" s="29" t="s">
         <v>42</v>
@@ -7566,13 +8354,13 @@
         <v>779</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>6</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -7589,10 +8377,10 @@
         <v>9</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="G23" s="28" t="s">
         <v>774</v>
@@ -7604,7 +8392,7 @@
         <v>9</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -7636,7 +8424,7 @@
         <v>283</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -7653,10 +8441,10 @@
         <v>76</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="G25" s="28" t="s">
         <v>774</v>
@@ -7668,7 +8456,7 @@
         <v>76</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -7685,10 +8473,10 @@
         <v>6</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="G26" s="28" t="s">
         <v>774</v>
@@ -7700,7 +8488,7 @@
         <v>6</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -7726,7 +8514,7 @@
         <v>6</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -7752,7 +8540,7 @@
         <v>6</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -7769,10 +8557,10 @@
         <v>9</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="F29" s="28" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="G29" s="28" t="s">
         <v>774</v>
@@ -7784,7 +8572,7 @@
         <v>9</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -7801,10 +8589,10 @@
         <v>9</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="F30" s="28" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="G30" s="28" t="s">
         <v>774</v>
@@ -7816,7 +8604,7 @@
         <v>9</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -7848,7 +8636,7 @@
         <v>283</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -7880,15 +8668,15 @@
         <v>76</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E33" s="28" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="F33" s="28" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="G33" s="28" t="s">
         <v>774</v>
@@ -7899,22 +8687,22 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -7924,48 +8712,48 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="21" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="23" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="20" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="23" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="23" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
@@ -7973,37 +8761,37 @@
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="24" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="23" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="32" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
anonymization update: new UID generation + default/shanoir anonymization + code de keep some tags non anominized to allow OFSEP/neurinfo profiles
</commit_message>
<xml_diff>
--- a/shanoir-ng-import/src/main/resources/anonymization.xlsx
+++ b/shanoir-ng-import/src/main/resources/anonymization.xlsx
@@ -3,20 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ifakhfak\Documents\Shanoir NG\Import MS\Anomymization Spec\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14100" windowHeight="6675"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A286:E299"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="821">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="820">
   <si>
     <t>Attribute Name</t>
   </si>
@@ -2594,9 +2590,6 @@
     </r>
   </si>
   <si>
-    <t>Z if no contrast agent is used, otherwise D</t>
-  </si>
-  <si>
     <r>
       <t>IODs and SOP Classes define Type 2C elements that have</t>
     </r>
@@ -2623,10 +2616,10 @@
     <t>X because we are uploading patients not animals. Moreover the module "Patient Study" is a User option</t>
   </si>
   <si>
-    <t>Z ?</t>
-  </si>
-  <si>
     <t>MR Profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z </t>
   </si>
 </sst>
 </file>
@@ -3144,8 +3137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E305"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="B141" workbookViewId="0">
+      <selection activeCell="E150" sqref="E150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3171,7 +3164,7 @@
         <v>409</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3728,7 +3721,7 @@
         <v>48</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -5395,7 +5388,7 @@
         <v>4</v>
       </c>
       <c r="E150" s="9" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -7824,7 +7817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView topLeftCell="D19" workbookViewId="0">
+    <sheetView topLeftCell="I10" workbookViewId="0">
       <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
@@ -8096,7 +8089,7 @@
         <v>48</v>
       </c>
       <c r="K11" s="31" t="s">
-        <v>816</v>
+        <v>819</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -8360,7 +8353,7 @@
         <v>6</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -8766,7 +8759,7 @@
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="23" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>